<commit_message>
Add tests for simple xlsb
</commit_message>
<xml_diff>
--- a/OOXML/test/ExampleFiles/xlsx2xlsb/simple1.xlsx
+++ b/OOXML/test/ExampleFiles/xlsx2xlsb/simple1.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr allowRefreshQuery="0" autoCompressPictures="1" backupFile="0" checkCompatibility="0" codeName="0" date1904="0" dateCompatibility="1" defaultThemeVersion="0" filterPrivacy="0" hidePivotFieldList="0" promptedSolutions="0" publishItems="0" refreshAllConnections="0" showBorderUnselectedTables="0" showInkAnnotation="1" showObjects="all" showPivotChartFilter="0" updateLinks="always"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF3FA02E-C34F-4E97-A5AF-9322D362F4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcMode="autoNoTable" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001" fullPrecision="1" calcCompleted="0" calcOnSave="1" concurrentCalc="1" concurrentManualCount="1" forceFullCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -21,90 +28,63 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <i val="0"/>
-      <strike val="0"/>
-      <condense val="0"/>
-      <extend val="0"/>
-      <outline val="0"/>
-      <shadow val="0"/>
-      <u val="none"/>
-      <vertAlign val="baseline"/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
     <border>
-      <left style="none">
-        <color auto="1"/>
-      </left>
-      <right style="none">
-        <color auto="1"/>
-      </right>
-      <top style="none">
-        <color auto="1"/>
-      </top>
-      <bottom style="none">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none">
-        <color auto="1"/>
-      </diagonal>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="general" indent="0" justifyLastLine="0" readingOrder="0" relativeIndent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43E5-95BD-54CBDDF9020C}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -300,24 +280,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr syncHorizontal="0" syncVertical="0" transitionEvaluation="0" transitionEntry="0" published="1" filterMode="0" enableFormatConditionsCalculation="0">
-    <tabColor auto="1"/>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C4:D4"/>
   <sheetViews>
-    <sheetView windowProtection="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" showWhiteSpace="0" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="4" ht="14.5">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>1</v>
       </c>
@@ -326,9 +303,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="0" autoFilter="0" content="1" deleteColumns="0" deleteRows="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" insertRows="0" objects="1" pivotTables="0" scenarios="1" selectLockedCells="1" selectUnlockedCells="1" sheet="0" sort="0"/>
-  <printOptions headings="0" gridLines="0" gridLinesSet="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1" r:id=""/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>